<commit_message>
Changed 1883 to 1993 for witch str_yrs
</commit_message>
<xml_diff>
--- a/Data/DR_Stocks/Advice_Sheets/stock_metadata_refpts.xlsx
+++ b/Data/DR_Stocks/Advice_Sheets/stock_metadata_refpts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefas-my.sharepoint.com/personal/peter_kidd_cefas_gov_uk/Documents/Projects/C8503B/PhD/DATRAS/Spatial Indicator R Project/Stocks/Advice Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefas-my.sharepoint.com/personal/peter_kidd_cefas_gov_uk/Documents/Projects/C8503B/PhD/SpatIndAssess(GIT)/SpatIndAssess/Data/DR_Stocks/Advice_Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{A8FB5902-299E-49A2-BD1E-0FEA1BCA3EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58B51FA2-E8A6-49B5-B63C-7B728283D489}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{A8FB5902-299E-49A2-BD1E-0FEA1BCA3EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC572F99-C454-4A87-8DC3-FD3BFA43698E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F2B49E6A-08D5-481B-9D34-DE9AC72A6B55}"/>
   </bookViews>
@@ -4260,7 +4260,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5291,7 +5291,7 @@
         <v>36</v>
       </c>
       <c r="I30">
-        <v>1883</v>
+        <v>1983</v>
       </c>
       <c r="K30">
         <v>1</v>

</xml_diff>